<commit_message>
fixed #190 FlixelRL-190 Floor1〜3: 敵の強さの調整
</commit_message>
<xml_diff>
--- a/docs/player.xlsx
+++ b/docs/player.xlsx
@@ -1399,7 +1399,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.13281" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.13281" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.55469" style="1" customWidth="1"/>
     <col min="5" max="5" width="4.64062" style="1" customWidth="1"/>
@@ -1460,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -1478,7 +1478,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -1499,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5">
         <v>3</v>
@@ -1520,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -1541,7 +1541,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C7" s="5">
         <v>4</v>
@@ -1562,7 +1562,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="C8" s="5">
         <v>5</v>
@@ -1583,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="5">
-        <v>100</v>
+        <v>800</v>
       </c>
       <c r="C9" s="5">
         <v>5</v>
@@ -1604,7 +1604,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="C10" s="5">
         <v>5</v>
@@ -1625,7 +1625,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5">
-        <v>450</v>
+        <v>1800</v>
       </c>
       <c r="C11" s="5">
         <v>5</v>
@@ -1646,7 +1646,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="5">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="C12" s="5">
         <v>5</v>
@@ -1667,7 +1667,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5">
-        <v>550</v>
+        <v>5000</v>
       </c>
       <c r="C13" s="5">
         <v>5</v>
@@ -1688,7 +1688,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="5">
-        <v>600</v>
+        <v>10000</v>
       </c>
       <c r="C14" s="5">
         <v>5</v>
@@ -1709,7 +1709,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>650</v>
+        <v>30000</v>
       </c>
       <c r="C15" s="5">
         <v>5</v>
@@ -1730,7 +1730,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>700</v>
+        <v>50000</v>
       </c>
       <c r="C16" s="5">
         <v>5</v>
@@ -1751,7 +1751,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>750</v>
+        <v>80000</v>
       </c>
       <c r="C17" s="5">
         <v>144</v>
@@ -1772,7 +1772,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>800</v>
+        <v>120000</v>
       </c>
       <c r="C18" s="5">
         <v>152</v>
@@ -1793,7 +1793,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>850</v>
+        <v>170000</v>
       </c>
       <c r="C19" s="5">
         <v>160</v>
@@ -1814,7 +1814,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>900</v>
+        <v>250000</v>
       </c>
       <c r="C20" s="5">
         <v>168</v>
@@ -1835,7 +1835,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="5">
-        <v>950</v>
+        <v>500000</v>
       </c>
       <c r="C21" s="5">
         <v>176</v>
@@ -1856,7 +1856,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="5">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="C22" s="5">
         <v>184</v>
@@ -1877,7 +1877,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="5">
-        <v>1050</v>
+        <v>2000000</v>
       </c>
       <c r="C23" s="5">
         <v>192</v>
@@ -1898,7 +1898,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="5">
-        <v>1100</v>
+        <v>3000000</v>
       </c>
       <c r="C24" s="5">
         <v>200</v>
@@ -1919,7 +1919,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="5">
-        <v>1150</v>
+        <v>4000000</v>
       </c>
       <c r="C25" s="5">
         <v>208</v>
@@ -1940,7 +1940,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="5">
-        <v>1200</v>
+        <v>5000000</v>
       </c>
       <c r="C26" s="5">
         <v>216</v>
@@ -1961,7 +1961,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="5">
-        <v>1250</v>
+        <v>6000000</v>
       </c>
       <c r="C27" s="5">
         <v>224</v>
@@ -1982,7 +1982,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="5">
-        <v>1300</v>
+        <v>7000000</v>
       </c>
       <c r="C28" s="5">
         <v>232</v>
@@ -2003,7 +2003,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="5">
-        <v>1350</v>
+        <v>8000000</v>
       </c>
       <c r="C29" s="5">
         <v>240</v>
@@ -2024,7 +2024,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="5">
-        <v>1400</v>
+        <v>9000000</v>
       </c>
       <c r="C30" s="5">
         <v>248</v>
@@ -2045,7 +2045,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="5">
-        <v>1450</v>
+        <v>10000000</v>
       </c>
       <c r="C31" s="5">
         <v>256</v>
@@ -2066,7 +2066,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="5">
-        <v>1500</v>
+        <v>11000000</v>
       </c>
       <c r="C32" s="5">
         <v>264</v>
@@ -2087,7 +2087,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="5">
-        <v>1550</v>
+        <v>12000000</v>
       </c>
       <c r="C33" s="5">
         <v>272</v>
@@ -2108,7 +2108,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="5">
-        <v>1600</v>
+        <v>13000000</v>
       </c>
       <c r="C34" s="5">
         <v>280</v>
@@ -2129,7 +2129,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="5">
-        <v>1650</v>
+        <v>14000000</v>
       </c>
       <c r="C35" s="5">
         <v>288</v>
@@ -2150,7 +2150,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="5">
-        <v>1700</v>
+        <v>15000000</v>
       </c>
       <c r="C36" s="5">
         <v>296</v>
@@ -2171,7 +2171,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="5">
-        <v>1750</v>
+        <v>16000000</v>
       </c>
       <c r="C37" s="5">
         <v>304</v>
@@ -2192,7 +2192,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="5">
-        <v>1800</v>
+        <v>17000000</v>
       </c>
       <c r="C38" s="5">
         <v>312</v>
@@ -2213,7 +2213,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="5">
-        <v>1850</v>
+        <v>18000000</v>
       </c>
       <c r="C39" s="5">
         <v>320</v>
@@ -2234,7 +2234,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="5">
-        <v>1900</v>
+        <v>19000000</v>
       </c>
       <c r="C40" s="5">
         <v>328</v>
@@ -2255,7 +2255,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="5">
-        <v>1950</v>
+        <v>20000000</v>
       </c>
       <c r="C41" s="5">
         <v>336</v>
@@ -2276,7 +2276,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="5">
-        <v>2000</v>
+        <v>21000000</v>
       </c>
       <c r="C42" s="5">
         <v>344</v>
@@ -2297,7 +2297,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="5">
-        <v>2050</v>
+        <v>22000000</v>
       </c>
       <c r="C43" s="5">
         <v>352</v>
@@ -2318,7 +2318,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="5">
-        <v>2100</v>
+        <v>23000000</v>
       </c>
       <c r="C44" s="5">
         <v>360</v>
@@ -2339,7 +2339,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="5">
-        <v>2150</v>
+        <v>24000000</v>
       </c>
       <c r="C45" s="5">
         <v>368</v>
@@ -2360,7 +2360,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="5">
-        <v>2200</v>
+        <v>25000000</v>
       </c>
       <c r="C46" s="5">
         <v>376</v>
@@ -2381,7 +2381,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="5">
-        <v>2250</v>
+        <v>26000000</v>
       </c>
       <c r="C47" s="5">
         <v>384</v>
@@ -2402,7 +2402,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="5">
-        <v>2300</v>
+        <v>27000000</v>
       </c>
       <c r="C48" s="5">
         <v>392</v>
@@ -2423,7 +2423,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="5">
-        <v>2350</v>
+        <v>28000000</v>
       </c>
       <c r="C49" s="5">
         <v>400</v>
@@ -2444,7 +2444,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="5">
-        <v>2400</v>
+        <v>29000000</v>
       </c>
       <c r="C50" s="5">
         <v>408</v>
@@ -2465,7 +2465,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="5">
-        <v>2450</v>
+        <v>30000000</v>
       </c>
       <c r="C51" s="5">
         <v>416</v>
@@ -2486,7 +2486,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="5">
-        <v>2500</v>
+        <v>31000000</v>
       </c>
       <c r="C52" s="5">
         <v>424</v>
@@ -2507,7 +2507,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="5">
-        <v>2550</v>
+        <v>32000000</v>
       </c>
       <c r="C53" s="5">
         <v>432</v>
@@ -2528,7 +2528,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="5">
-        <v>2600</v>
+        <v>33000000</v>
       </c>
       <c r="C54" s="5">
         <v>440</v>
@@ -2549,7 +2549,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="5">
-        <v>2650</v>
+        <v>34000000</v>
       </c>
       <c r="C55" s="5">
         <v>448</v>
@@ -2570,7 +2570,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="5">
-        <v>2700</v>
+        <v>35000000</v>
       </c>
       <c r="C56" s="5">
         <v>456</v>
@@ -2591,7 +2591,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="5">
-        <v>2750</v>
+        <v>36000000</v>
       </c>
       <c r="C57" s="5">
         <v>464</v>
@@ -2612,7 +2612,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="5">
-        <v>2800</v>
+        <v>37000000</v>
       </c>
       <c r="C58" s="5">
         <v>472</v>
@@ -2633,7 +2633,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="5">
-        <v>2850</v>
+        <v>38000000</v>
       </c>
       <c r="C59" s="5">
         <v>480</v>
@@ -2654,7 +2654,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="5">
-        <v>2900</v>
+        <v>39000000</v>
       </c>
       <c r="C60" s="5">
         <v>488</v>
@@ -2675,7 +2675,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="5">
-        <v>2950</v>
+        <v>40000000</v>
       </c>
       <c r="C61" s="5">
         <v>496</v>
@@ -2696,7 +2696,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="5">
-        <v>3000</v>
+        <v>41000000</v>
       </c>
       <c r="C62" s="5">
         <v>504</v>
@@ -2717,7 +2717,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="5">
-        <v>3050</v>
+        <v>42000000</v>
       </c>
       <c r="C63" s="5">
         <v>512</v>
@@ -2738,7 +2738,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="5">
-        <v>3100</v>
+        <v>43000000</v>
       </c>
       <c r="C64" s="5">
         <v>520</v>
@@ -2759,7 +2759,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="5">
-        <v>3150</v>
+        <v>44000000</v>
       </c>
       <c r="C65" s="5">
         <v>528</v>
@@ -2780,7 +2780,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="5">
-        <v>3200</v>
+        <v>45000000</v>
       </c>
       <c r="C66" s="5">
         <v>536</v>
@@ -2801,7 +2801,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="5">
-        <v>3250</v>
+        <v>46000000</v>
       </c>
       <c r="C67" s="5">
         <v>544</v>
@@ -2822,7 +2822,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="5">
-        <v>3300</v>
+        <v>47000000</v>
       </c>
       <c r="C68" s="5">
         <v>552</v>
@@ -2843,7 +2843,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="5">
-        <v>3350</v>
+        <v>48000000</v>
       </c>
       <c r="C69" s="5">
         <v>560</v>
@@ -2864,7 +2864,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="5">
-        <v>3400</v>
+        <v>49000000</v>
       </c>
       <c r="C70" s="5">
         <v>568</v>
@@ -2885,7 +2885,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="5">
-        <v>3450</v>
+        <v>50000000</v>
       </c>
       <c r="C71" s="5">
         <v>576</v>
@@ -2906,7 +2906,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="5">
-        <v>3500</v>
+        <v>51000000</v>
       </c>
       <c r="C72" s="5">
         <v>584</v>
@@ -2927,7 +2927,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="5">
-        <v>3550</v>
+        <v>52000000</v>
       </c>
       <c r="C73" s="5">
         <v>592</v>
@@ -2948,7 +2948,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="5">
-        <v>3600</v>
+        <v>53000000</v>
       </c>
       <c r="C74" s="5">
         <v>600</v>
@@ -2969,7 +2969,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="5">
-        <v>3650</v>
+        <v>54000000</v>
       </c>
       <c r="C75" s="5">
         <v>608</v>
@@ -2990,7 +2990,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="5">
-        <v>3700</v>
+        <v>55000000</v>
       </c>
       <c r="C76" s="5">
         <v>616</v>
@@ -3011,7 +3011,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="5">
-        <v>3750</v>
+        <v>56000000</v>
       </c>
       <c r="C77" s="5">
         <v>624</v>
@@ -3032,7 +3032,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="5">
-        <v>3800</v>
+        <v>57000000</v>
       </c>
       <c r="C78" s="5">
         <v>632</v>
@@ -3053,7 +3053,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="5">
-        <v>3850</v>
+        <v>58000000</v>
       </c>
       <c r="C79" s="5">
         <v>640</v>
@@ -3074,7 +3074,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="5">
-        <v>3900</v>
+        <v>59000000</v>
       </c>
       <c r="C80" s="5">
         <v>648</v>
@@ -3095,7 +3095,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="5">
-        <v>3950</v>
+        <v>60000000</v>
       </c>
       <c r="C81" s="5">
         <v>656</v>
@@ -3116,7 +3116,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="5">
-        <v>4000</v>
+        <v>61000000</v>
       </c>
       <c r="C82" s="5">
         <v>664</v>
@@ -3137,7 +3137,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="5">
-        <v>4050</v>
+        <v>62000000</v>
       </c>
       <c r="C83" s="5">
         <v>672</v>
@@ -3158,7 +3158,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="5">
-        <v>4100</v>
+        <v>63000000</v>
       </c>
       <c r="C84" s="5">
         <v>680</v>
@@ -3179,7 +3179,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="5">
-        <v>4150</v>
+        <v>64000000</v>
       </c>
       <c r="C85" s="5">
         <v>688</v>
@@ -3200,7 +3200,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="5">
-        <v>4200</v>
+        <v>65000000</v>
       </c>
       <c r="C86" s="5">
         <v>696</v>
@@ -3221,7 +3221,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="5">
-        <v>4250</v>
+        <v>66000000</v>
       </c>
       <c r="C87" s="5">
         <v>704</v>
@@ -3242,7 +3242,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="5">
-        <v>4300</v>
+        <v>67000000</v>
       </c>
       <c r="C88" s="5">
         <v>712</v>
@@ -3263,7 +3263,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="5">
-        <v>4350</v>
+        <v>68000000</v>
       </c>
       <c r="C89" s="5">
         <v>720</v>
@@ -3284,7 +3284,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="5">
-        <v>4400</v>
+        <v>69000000</v>
       </c>
       <c r="C90" s="5">
         <v>728</v>
@@ -3305,7 +3305,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="5">
-        <v>4450</v>
+        <v>70000000</v>
       </c>
       <c r="C91" s="5">
         <v>736</v>
@@ -3326,7 +3326,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="5">
-        <v>4500</v>
+        <v>71000000</v>
       </c>
       <c r="C92" s="5">
         <v>744</v>
@@ -3347,7 +3347,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="5">
-        <v>4550</v>
+        <v>72000000</v>
       </c>
       <c r="C93" s="5">
         <v>752</v>
@@ -3368,7 +3368,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="5">
-        <v>4600</v>
+        <v>73000000</v>
       </c>
       <c r="C94" s="5">
         <v>760</v>
@@ -3389,7 +3389,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="5">
-        <v>4650</v>
+        <v>74000000</v>
       </c>
       <c r="C95" s="5">
         <v>768</v>
@@ -3410,7 +3410,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="5">
-        <v>4700</v>
+        <v>75000000</v>
       </c>
       <c r="C96" s="5">
         <v>776</v>
@@ -3431,7 +3431,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="5">
-        <v>4750</v>
+        <v>76000000</v>
       </c>
       <c r="C97" s="5">
         <v>784</v>
@@ -3452,7 +3452,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="5">
-        <v>4800</v>
+        <v>77000000</v>
       </c>
       <c r="C98" s="5">
         <v>792</v>
@@ -3473,7 +3473,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="5">
-        <v>4850</v>
+        <v>78000000</v>
       </c>
       <c r="C99" s="5">
         <v>800</v>
@@ -3494,7 +3494,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="5">
-        <v>4900</v>
+        <v>79000000</v>
       </c>
       <c r="C100" s="5">
         <v>808</v>
@@ -3515,7 +3515,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="5">
-        <v>4950</v>
+        <v>80000000</v>
       </c>
       <c r="C101" s="5">
         <v>816</v>
@@ -3536,7 +3536,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="5">
-        <v>5000</v>
+        <v>81000000</v>
       </c>
       <c r="C102" s="5">
         <v>999</v>

</xml_diff>